<commit_message>
Added first input validations
</commit_message>
<xml_diff>
--- a/expense_tracker/expenses.xlsx
+++ b/expense_tracker/expenses.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git repos\personal_projects\expense_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F6E0B6-E5E0-4D2F-B842-138E0C2F106D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB66BAF-D2D2-490D-86F5-7C8B7EC692DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -30,7 +25,7 @@
     <t>Items</t>
   </si>
   <si>
-    <t>Total cost</t>
+    <t>Cost</t>
   </si>
   <si>
     <t>Date</t>
@@ -354,12 +349,14 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>